<commit_message>
Updated NotificationController with distinguishable PendingIntent RequestCodes
</commit_message>
<xml_diff>
--- a/Documentation/Work-Time.xlsx
+++ b/Documentation/Work-Time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\Android_Apps\Notification-Demo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AA9349-B7F1-40D1-B0E6-12A70BCC60F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CD8B05-D1D1-4550-8787-EE70B197F990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <t>Datum</t>
   </si>
   <si>
-    <t>Zeit</t>
+    <t>Zeit in h</t>
   </si>
 </sst>
 </file>
@@ -109,12 +109,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -397,28 +398,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>44424</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating UI and starting to implement DirectReply
</commit_message>
<xml_diff>
--- a/Documentation/Work-Time.xlsx
+++ b/Documentation/Work-Time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\Android_Apps\Notification-Demo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CD8B05-D1D1-4550-8787-EE70B197F990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB6AD6B-C53A-448D-8146-DDF7AF012D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -76,32 +76,47 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
-      <top style="thick">
-        <color auto="1"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="thick">
-        <color auto="1"/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
-      <right style="thick">
-        <color auto="1"/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
-      <top style="thick">
-        <color auto="1"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom style="thick">
-        <color auto="1"/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -109,13 +124,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -396,29 +413,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="A3:B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>44424</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>44437</v>
+      </c>
+      <c r="B3" s="5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arbeitszeit und Plan modifiziert
</commit_message>
<xml_diff>
--- a/Documentation/Work-Time.xlsx
+++ b/Documentation/Work-Time.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten\Android_Apps\Notification-Demo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB6AD6B-C53A-448D-8146-DDF7AF012D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B23C75-B41D-4FCA-B090-4F6CED68589C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Datum</t>
   </si>
   <si>
     <t>Zeit in h</t>
+  </si>
+  <si>
+    <t>Issues schreiben und Planen</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:B3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +427,7 @@
     <col min="1" max="1" width="10.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -432,7 +435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44424</v>
       </c>
@@ -440,12 +443,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>44437</v>
       </c>
       <c r="B3" s="5">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>44467</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>